<commit_message>
udpate example test case
</commit_message>
<xml_diff>
--- a/tests/component/update_student_sheets/test_cases/more_complexe_case/teacher.xlsx
+++ b/tests/component/update_student_sheets/test_cases/more_complexe_case/teacher.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsha\Documents\Git\student-teacher-gradebook\__tests__\component\update_student_sheets\test_cases\more_complexe_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsha\Documents\Git\student-teacher-gradebook\tests\component\update_student_sheets\test_cases\more_complexe_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E07B8A-8335-4769-B7BA-8AA7BB030755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B3CA9-2CD6-4724-B472-A5A4396A9989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{1C66C71B-6ED8-4699-9FB2-CB3156D48D4F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Student</t>
   </si>
@@ -130,9 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +503,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,21 +671,43 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D4DC52-0972-4CD9-A404-A48552193F94}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1">
         <v>57</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>